<commit_message>
Retry implementation fetching data
</commit_message>
<xml_diff>
--- a/data/gold/breweries_agg.xlsx
+++ b/data/gold/breweries_agg.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -927,7 +927,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37">
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41">
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>56</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2420</v>
+        <v>7260</v>
       </c>
     </row>
     <row r="47">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>245</v>
+        <v>735</v>
       </c>
     </row>
     <row r="62">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>188</v>
+        <v>564</v>
       </c>
     </row>
     <row r="77">
@@ -1587,7 +1587,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81">
@@ -1647,7 +1647,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>74</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92">
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107">
@@ -2052,7 +2052,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>40</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109">
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110">
@@ -2097,7 +2097,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>49</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113">
@@ -2127,7 +2127,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114">
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115">
@@ -2157,7 +2157,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="116">
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="117">
@@ -2187,7 +2187,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="118">
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="120">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="121">
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>4161</v>
+        <v>12483</v>
       </c>
     </row>
     <row r="122">
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123">
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129">
@@ -2472,7 +2472,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="137">
@@ -2697,7 +2697,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>674</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="152">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>69</v>
+        <v>207</v>
       </c>
     </row>
     <row r="167">
@@ -2997,7 +2997,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="172">
@@ -3027,7 +3027,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174">
@@ -3057,7 +3057,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="176">
@@ -3147,7 +3147,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>215</v>
+        <v>645</v>
       </c>
     </row>
     <row r="182">
@@ -3177,7 +3177,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="184">
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>